<commit_message>
Deploying to gh-pages from  @ 2692059376593b4bd0b9b460ed68f8b7954b89f5 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/16.2.2.xlsx
+++ b/en/downloads/data-excel/16.2.2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="40">
   <si>
     <t>Көрсөткүчтөрдүн аталышы</t>
   </si>
@@ -140,9 +140,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0"/>
-  </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -255,7 +252,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -297,38 +294,29 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -635,7 +623,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M27"/>
+  <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -646,7 +634,7 @@
     <col min="7" max="12" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>37</v>
       </c>
@@ -666,7 +654,7 @@
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>35</v>
       </c>
@@ -680,10 +668,10 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
     </row>
-    <row r="3" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
     </row>
-    <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>0</v>
       </c>
@@ -723,403 +711,454 @@
       <c r="M4" s="9">
         <v>2019</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" s="12" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="27" t="s">
+      <c r="N4" s="9">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" s="12" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
         <v>38</v>
       </c>
       <c r="B5" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="17">
+      <c r="D5" s="20">
         <v>21</v>
       </c>
-      <c r="E5" s="17">
+      <c r="E5" s="20">
         <v>5</v>
       </c>
-      <c r="F5" s="17">
+      <c r="F5" s="20">
         <v>6</v>
       </c>
-      <c r="G5" s="17">
+      <c r="G5" s="20">
         <v>9</v>
       </c>
-      <c r="H5" s="17">
+      <c r="H5" s="20">
         <v>19</v>
       </c>
-      <c r="I5" s="17">
+      <c r="I5" s="20">
         <v>8</v>
       </c>
-      <c r="J5" s="17">
+      <c r="J5" s="20">
         <v>10</v>
       </c>
-      <c r="K5" s="17">
+      <c r="K5" s="20">
         <v>5</v>
       </c>
-      <c r="L5" s="17">
+      <c r="L5" s="20">
         <v>8</v>
       </c>
-      <c r="M5" s="17">
+      <c r="M5" s="20">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
+      <c r="N5" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="F6" s="20">
-        <v>1</v>
-      </c>
-      <c r="G6" s="20">
+      <c r="D6" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="22">
+        <v>1</v>
+      </c>
+      <c r="G6" s="22">
         <v>2</v>
       </c>
-      <c r="H6" s="20">
-        <v>1</v>
-      </c>
-      <c r="I6" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="J6" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="K6" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="L6" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="M6" s="21"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
+      <c r="H6" s="22">
+        <v>1</v>
+      </c>
+      <c r="I6" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="J6" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="K6" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="L6" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="M6" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="N6" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="F7" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="G7" s="19">
-        <v>1</v>
-      </c>
-      <c r="H7" s="19">
-        <v>1</v>
-      </c>
-      <c r="I7" s="19">
-        <v>1</v>
-      </c>
-      <c r="J7" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="K7" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="L7" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="M7" s="22"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
+      <c r="D7" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" s="21">
+        <v>1</v>
+      </c>
+      <c r="H7" s="21">
+        <v>1</v>
+      </c>
+      <c r="I7" s="21">
+        <v>1</v>
+      </c>
+      <c r="J7" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="K7" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="L7" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="M7" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="N7" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="F8" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="G8" s="19">
-        <v>1</v>
-      </c>
-      <c r="H8" s="19">
-        <v>1</v>
-      </c>
-      <c r="I8" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="J8" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="K8" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="L8" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="M8" s="22"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
+      <c r="D8" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="21">
+        <v>1</v>
+      </c>
+      <c r="H8" s="21">
+        <v>1</v>
+      </c>
+      <c r="I8" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="J8" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="K8" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="L8" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="M8" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="N8" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="E9" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="F9" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="G9" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="H9" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="I9" s="19">
-        <v>1</v>
-      </c>
-      <c r="J9" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="K9" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="L9" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="M9" s="22"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
+      <c r="D9" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="H9" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="I9" s="21">
+        <v>1</v>
+      </c>
+      <c r="J9" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="K9" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="L9" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="M9" s="21">
+        <v>1</v>
+      </c>
+      <c r="N9" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="20">
+      <c r="D10" s="22">
         <v>5</v>
       </c>
-      <c r="E10" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="F10" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="G10" s="19">
-        <v>1</v>
-      </c>
-      <c r="H10" s="19">
+      <c r="E10" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" s="21">
+        <v>1</v>
+      </c>
+      <c r="H10" s="21">
         <v>6</v>
       </c>
-      <c r="I10" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="J10" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="K10" s="19">
+      <c r="I10" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="J10" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="K10" s="21">
         <v>2</v>
       </c>
-      <c r="L10" s="19">
-        <v>1</v>
-      </c>
-      <c r="M10" s="22"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="18" t="s">
+      <c r="L10" s="21">
+        <v>1</v>
+      </c>
+      <c r="M10" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="N10" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="E11" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="F11" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="G11" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="H11" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="I11" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="J11" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="K11" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="L11" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="M11" s="22"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="18" t="s">
+      <c r="D11" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="H11" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="I11" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="J11" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="K11" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="L11" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="M11" s="21">
+        <v>1</v>
+      </c>
+      <c r="N11" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="20">
+      <c r="D12" s="22">
         <v>2</v>
       </c>
-      <c r="E12" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="F12" s="20">
+      <c r="E12" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" s="22">
         <v>2</v>
       </c>
-      <c r="G12" s="20">
-        <v>3</v>
-      </c>
-      <c r="H12" s="20">
-        <v>3</v>
-      </c>
-      <c r="I12" s="20">
-        <v>3</v>
-      </c>
-      <c r="J12" s="20">
+      <c r="G12" s="22">
+        <v>3</v>
+      </c>
+      <c r="H12" s="22">
+        <v>3</v>
+      </c>
+      <c r="I12" s="22">
+        <v>3</v>
+      </c>
+      <c r="J12" s="22">
         <v>6</v>
       </c>
-      <c r="K12" s="20">
-        <v>3</v>
-      </c>
-      <c r="L12" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="M12" s="22"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
+      <c r="K12" s="22">
+        <v>3</v>
+      </c>
+      <c r="L12" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="M12" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="N12" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="20">
-        <v>1</v>
-      </c>
-      <c r="E13" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="F13" s="19">
-        <v>3</v>
-      </c>
-      <c r="G13" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="H13" s="19">
+      <c r="D13" s="22">
+        <v>1</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13" s="21">
+        <v>3</v>
+      </c>
+      <c r="G13" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="H13" s="21">
         <v>2</v>
       </c>
-      <c r="I13" s="19">
-        <v>1</v>
-      </c>
-      <c r="J13" s="19">
+      <c r="I13" s="21">
+        <v>1</v>
+      </c>
+      <c r="J13" s="21">
         <v>4</v>
       </c>
-      <c r="K13" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="L13" s="19">
+      <c r="K13" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="L13" s="21">
         <v>7</v>
       </c>
-      <c r="M13" s="22"/>
-    </row>
-    <row r="14" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="23" t="s">
+      <c r="M13" s="21">
+        <v>2</v>
+      </c>
+      <c r="N13" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="23" t="s">
+      <c r="C14" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="24">
+      <c r="D14" s="23">
         <v>13</v>
       </c>
-      <c r="E14" s="24">
+      <c r="E14" s="23">
         <v>5</v>
       </c>
-      <c r="F14" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="G14" s="25">
-        <v>1</v>
-      </c>
-      <c r="H14" s="25">
+      <c r="F14" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="G14" s="24">
+        <v>1</v>
+      </c>
+      <c r="H14" s="24">
         <v>5</v>
       </c>
-      <c r="I14" s="25">
+      <c r="I14" s="24">
         <v>2</v>
       </c>
-      <c r="J14" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="K14" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="L14" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="M14" s="26"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="J14" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="K14" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="L14" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="M14" s="24">
+        <v>1</v>
+      </c>
+      <c r="N14" s="24" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B15" s="11"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B16" s="11"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>